<commit_message>
HW2 updated - 08/05/17.
</commit_message>
<xml_diff>
--- a/TO DO list.xlsx
+++ b/TO DO list.xlsx
@@ -27,10 +27,10 @@
     <t>מה</t>
   </si>
   <si>
-    <t>דור</t>
+    <t>דור ושירה</t>
   </si>
   <si>
-    <t>ליצור את הרשימה הזו</t>
+    <t>שורה 1195 sched.c לשאול את העתיד</t>
   </si>
 </sst>
 </file>
@@ -392,10 +392,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>